<commit_message>
create group on the fly
</commit_message>
<xml_diff>
--- a/backend/meta_data.xlsx
+++ b/backend/meta_data.xlsx
@@ -379,6 +379,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -405,12 +406,14 @@
       <sz val="10"/>
       <name val="AR PL KaitiM GB"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="AR PL KaitiM GB"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -471,7 +474,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -493,10 +496,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -584,13 +583,13 @@
   </sheetPr>
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F88" activeCellId="0" sqref="F88"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.66"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -648,7 +647,7 @@
       <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -659,7 +658,7 @@
       <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -670,7 +669,7 @@
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -681,7 +680,7 @@
       <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -692,7 +691,7 @@
       <c r="B9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -703,7 +702,7 @@
       <c r="B10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -714,7 +713,7 @@
       <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -725,7 +724,7 @@
       <c r="B12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -736,7 +735,7 @@
       <c r="B13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -802,7 +801,7 @@
       <c r="B19" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -813,7 +812,7 @@
       <c r="B20" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -824,7 +823,7 @@
       <c r="B21" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -894,7 +893,7 @@
       <c r="B27" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F27" s="4"/>
@@ -906,7 +905,7 @@
       <c r="B28" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F28" s="4"/>
@@ -918,10 +917,10 @@
       <c r="B29" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F29" s="6"/>
+      <c r="C29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="4"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
@@ -930,10 +929,10 @@
       <c r="B30" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E30" s="7"/>
+      <c r="C30" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="6"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
@@ -942,10 +941,10 @@
       <c r="B31" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" s="7"/>
+      <c r="C31" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="6"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
@@ -954,10 +953,10 @@
       <c r="B32" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C32" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32" s="6"/>
+      <c r="C32" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="4"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
@@ -966,10 +965,10 @@
       <c r="B33" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E33" s="6"/>
+      <c r="C33" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="4"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
@@ -978,10 +977,10 @@
       <c r="B34" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C34" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" s="6"/>
+      <c r="C34" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="4"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
@@ -990,7 +989,7 @@
       <c r="B35" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1001,7 +1000,7 @@
       <c r="B36" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1012,7 +1011,7 @@
       <c r="B37" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1023,7 +1022,7 @@
       <c r="B38" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1034,7 +1033,7 @@
       <c r="B39" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1045,7 +1044,7 @@
       <c r="B40" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1056,7 +1055,7 @@
       <c r="B41" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1067,7 +1066,7 @@
       <c r="B42" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1078,7 +1077,7 @@
       <c r="B43" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1089,7 +1088,7 @@
       <c r="B44" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C44" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1100,7 +1099,7 @@
       <c r="B45" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1111,7 +1110,7 @@
       <c r="B46" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C46" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1122,7 +1121,7 @@
       <c r="B47" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1133,7 +1132,7 @@
       <c r="B48" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C48" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1144,7 +1143,7 @@
       <c r="B49" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="C49" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1155,7 +1154,7 @@
       <c r="B50" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="C50" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1166,7 +1165,7 @@
       <c r="B51" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C51" s="6" t="s">
+      <c r="C51" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1177,7 +1176,7 @@
       <c r="B52" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C52" s="6" t="s">
+      <c r="C52" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1188,7 +1187,7 @@
       <c r="B53" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C53" s="6" t="s">
+      <c r="C53" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1199,7 +1198,7 @@
       <c r="B54" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C54" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1210,7 +1209,7 @@
       <c r="B55" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C55" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1221,7 +1220,7 @@
       <c r="B56" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="C56" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1232,7 +1231,7 @@
       <c r="B57" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C57" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1243,7 +1242,7 @@
       <c r="B58" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C58" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1254,7 +1253,7 @@
       <c r="B59" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C59" s="6" t="s">
+      <c r="C59" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1265,7 +1264,7 @@
       <c r="B60" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C60" s="6" t="s">
+      <c r="C60" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1276,7 +1275,7 @@
       <c r="B61" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="C61" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1287,7 +1286,7 @@
       <c r="B62" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="C62" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1298,7 +1297,7 @@
       <c r="B63" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="C63" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1309,7 +1308,7 @@
       <c r="B64" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C64" s="6" t="s">
+      <c r="C64" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1320,7 +1319,7 @@
       <c r="B65" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C65" s="6" t="s">
+      <c r="C65" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1331,7 +1330,7 @@
       <c r="B66" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C66" s="6" t="s">
+      <c r="C66" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1342,7 +1341,7 @@
       <c r="B67" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C67" s="6" t="s">
+      <c r="C67" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1353,7 +1352,7 @@
       <c r="B68" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C68" s="6" t="s">
+      <c r="C68" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1364,7 +1363,7 @@
       <c r="B69" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C69" s="6" t="s">
+      <c r="C69" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1375,7 +1374,7 @@
       <c r="B70" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C70" s="6" t="s">
+      <c r="C70" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1386,7 +1385,7 @@
       <c r="B71" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C71" s="6" t="s">
+      <c r="C71" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1397,7 +1396,7 @@
       <c r="B72" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C72" s="6" t="s">
+      <c r="C72" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1408,7 +1407,7 @@
       <c r="B73" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C73" s="6" t="s">
+      <c r="C73" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1419,7 +1418,7 @@
       <c r="B74" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C74" s="6" t="s">
+      <c r="C74" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1430,7 +1429,7 @@
       <c r="B75" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C75" s="6" t="s">
+      <c r="C75" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1441,7 +1440,7 @@
       <c r="B76" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C76" s="6" t="s">
+      <c r="C76" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1452,7 +1451,7 @@
       <c r="B77" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C77" s="6" t="s">
+      <c r="C77" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1463,7 +1462,7 @@
       <c r="B78" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C78" s="6" t="s">
+      <c r="C78" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1474,7 +1473,7 @@
       <c r="B79" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C79" s="6" t="s">
+      <c r="C79" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1485,7 +1484,7 @@
       <c r="B80" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C80" s="6" t="s">
+      <c r="C80" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1496,7 +1495,7 @@
       <c r="B81" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C81" s="6" t="s">
+      <c r="C81" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1507,7 +1506,7 @@
       <c r="B82" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C82" s="6" t="s">
+      <c r="C82" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1518,7 +1517,7 @@
       <c r="B83" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C83" s="6" t="s">
+      <c r="C83" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1529,7 +1528,7 @@
       <c r="B84" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C84" s="6" t="s">
+      <c r="C84" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1540,7 +1539,7 @@
       <c r="B85" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C85" s="6" t="s">
+      <c r="C85" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1551,7 +1550,7 @@
       <c r="B86" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C86" s="6" t="s">
+      <c r="C86" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1562,7 +1561,7 @@
       <c r="B87" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C87" s="6" t="s">
+      <c r="C87" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1573,7 +1572,7 @@
       <c r="B88" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C88" s="6" t="s">
+      <c r="C88" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1584,7 +1583,7 @@
       <c r="B89" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C89" s="6" t="s">
+      <c r="C89" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1595,7 +1594,7 @@
       <c r="B90" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C90" s="6" t="s">
+      <c r="C90" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1606,7 +1605,7 @@
       <c r="B91" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C91" s="6" t="s">
+      <c r="C91" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1617,7 +1616,7 @@
       <c r="B92" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C92" s="6" t="s">
+      <c r="C92" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1628,7 +1627,7 @@
       <c r="B93" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C93" s="6" t="s">
+      <c r="C93" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1639,7 +1638,7 @@
       <c r="B94" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C94" s="6" t="s">
+      <c r="C94" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1650,7 +1649,7 @@
       <c r="B95" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C95" s="6" t="s">
+      <c r="C95" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1661,7 +1660,7 @@
       <c r="B96" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C96" s="6" t="s">
+      <c r="C96" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1672,7 +1671,7 @@
       <c r="B97" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C97" s="6" t="s">
+      <c r="C97" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1683,7 +1682,7 @@
       <c r="B98" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C98" s="6" t="s">
+      <c r="C98" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1694,7 +1693,7 @@
       <c r="B99" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C99" s="6" t="s">
+      <c r="C99" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1705,7 +1704,7 @@
       <c r="B100" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C100" s="6" t="s">
+      <c r="C100" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1716,7 +1715,7 @@
       <c r="B101" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C101" s="6" t="s">
+      <c r="C101" s="4" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>